<commit_message>
Updated abstract, powerpoint, and spreadsheet
</commit_message>
<xml_diff>
--- a/Spreadsheets/feature_hists.xlsx
+++ b/Spreadsheets/feature_hists.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="trai_norm_email_features_100_0 " sheetId="1" r:id="rId1"/>
@@ -1292,12 +1292,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2109571712"/>
-        <c:axId val="2109579840"/>
-        <c:axId val="2109585472"/>
+        <c:axId val="2100260800"/>
+        <c:axId val="2100268928"/>
+        <c:axId val="2100274560"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2109571712"/>
+        <c:axId val="2100260800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1374,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109579840"/>
+        <c:crossAx val="2100268928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1382,7 +1382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109579840"/>
+        <c:axId val="2100268928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,12 +1451,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109571712"/>
+        <c:crossAx val="2100260800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2109585472"/>
+        <c:axId val="2100274560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,7 +1488,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109579840"/>
+        <c:crossAx val="2100268928"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2186,11 +2186,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2105793184"/>
-        <c:axId val="2105787216"/>
+        <c:axId val="2099378208"/>
+        <c:axId val="2099372240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105793184"/>
+        <c:axId val="2099378208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2289,7 +2289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2105787216"/>
+        <c:crossAx val="2099372240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2297,7 +2297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105787216"/>
+        <c:axId val="2099372240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2404,7 +2404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2105793184"/>
+        <c:crossAx val="2099378208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3179,12 +3179,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2109634624"/>
-        <c:axId val="2109640608"/>
-        <c:axId val="2109646720"/>
+        <c:axId val="2098735968"/>
+        <c:axId val="2098741952"/>
+        <c:axId val="2098748064"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2109634624"/>
+        <c:axId val="2098735968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3277,7 +3277,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109640608"/>
+        <c:crossAx val="2098741952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3285,7 +3285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109640608"/>
+        <c:axId val="2098741952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3392,12 +3392,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109634624"/>
+        <c:crossAx val="2098735968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2109646720"/>
+        <c:axId val="2098748064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3433,7 +3433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109640608"/>
+        <c:crossAx val="2098741952"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
       </c:serAx>
@@ -4131,11 +4131,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109094848"/>
-        <c:axId val="2109088896"/>
+        <c:axId val="2099262208"/>
+        <c:axId val="2099256256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109094848"/>
+        <c:axId val="2099262208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4234,7 +4234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109088896"/>
+        <c:crossAx val="2099256256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4242,7 +4242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109088896"/>
+        <c:axId val="2099256256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4349,7 +4349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109094848"/>
+        <c:crossAx val="2099262208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6157,8 +6157,8 @@
     <xdr:from>
       <xdr:col>33</xdr:col>
       <xdr:colOff>150090</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>2308</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
@@ -6451,7 +6451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView topLeftCell="P1" zoomScale="115" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
@@ -7789,8 +7789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView topLeftCell="Z8" zoomScale="125" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="AO34" sqref="AO34"/>
+    <sheetView tabSelected="1" topLeftCell="G15" zoomScale="125" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>